<commit_message>
semi conclusão do cap 3 e inicio do cap 4
</commit_message>
<xml_diff>
--- a/TCC/experimentos3/resultados/calibragemJanelaTreino.xlsx
+++ b/TCC/experimentos3/resultados/calibragemJanelaTreino.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="22260" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TentativaFiles" sheetId="1" r:id="rId1"/>
@@ -3534,6 +3534,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3621,9 +3622,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1130559004016632"/>
+          <c:x val="0.12380067139713921"/>
           <c:y val="3.7180657719806415E-2"/>
-          <c:w val="0.86068810583393951"/>
+          <c:w val="0.84886711476893362"/>
           <c:h val="0.80075078250476062"/>
         </c:manualLayout>
       </c:layout>
@@ -4565,7 +4566,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
@@ -4598,7 +4599,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
@@ -4636,7 +4637,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
@@ -4656,8 +4657,8 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
+        <c:tickLblSkip val="5"/>
+        <c:tickMarkSkip val="10"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -4688,7 +4689,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
@@ -4707,7 +4708,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="6.9358468200899775E-3"/>
+              <c:y val="0.36882942608050262"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4721,7 +4729,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
@@ -4753,7 +4761,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
@@ -4794,7 +4802,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22050777055342607"/>
+          <c:y val="0.94493518764054596"/>
+          <c:w val="0.55572368016511731"/>
+          <c:h val="5.5064812359454096E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4808,7 +4825,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
@@ -4848,7 +4865,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1050" b="1"/>
+        <a:defRPr sz="1400" b="1"/>
       </a:pPr>
       <a:endParaRPr lang="pt-BR"/>
     </a:p>
@@ -6034,16 +6051,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>300790</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>92868</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>168087</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>202046</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>98196</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>179293</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6330,7 +6347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="V11" zoomScale="80" zoomScaleNormal="25" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -13087,8 +13104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH192"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q13" zoomScale="44" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScale="20" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26562,6 +26579,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:S2"/>
@@ -26578,10 +26599,6 @@
     <mergeCell ref="N100:N101"/>
     <mergeCell ref="O100:S100"/>
     <mergeCell ref="T100:T101"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>